<commit_message>
I think I got it to work with an MFNN. I need to verify the graphs with the data from src/Output.txt.
</commit_message>
<xml_diff>
--- a/Outputs.xlsx
+++ b/Outputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\GitHub\deep-learning-for-indentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C48808C-81A4-422C-94AC-563FB868F94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF7658C-E2B4-43AB-9D86-D0F4FC173253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2D3233FC-92CD-487E-A53E-5AA3DA8C9992}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{2D3233FC-92CD-487E-A53E-5AA3DA8C9992}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="6">
   <si>
     <t>σy</t>
   </si>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4224C72D-A71F-4B68-9E93-BB5006E1018B}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,31 +450,31 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>7.38446376</v>
+        <v>34.080206910000001</v>
       </c>
       <c r="D2">
-        <v>1.3116536700000001</v>
+        <v>12.675873040000001</v>
       </c>
       <c r="E2">
-        <v>4.9361940500000001</v>
+        <v>19.31180367</v>
       </c>
       <c r="F2">
-        <v>1.74442096</v>
+        <v>2.2248757000000001</v>
       </c>
       <c r="G2">
-        <v>3.9482335700000002</v>
+        <v>22.805635580000001</v>
       </c>
       <c r="H2">
-        <v>0.65360253999999995</v>
+        <v>2.4222574300000002</v>
       </c>
       <c r="I2">
-        <v>3.86761577</v>
+        <v>5.2167098899999997</v>
       </c>
       <c r="J2">
-        <v>0.76814119999999997</v>
+        <v>0.48746171999999999</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -485,16 +485,252 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>33.274503660000001</v>
+        <v>25.995660770000001</v>
       </c>
       <c r="D3">
-        <v>13.40558776</v>
+        <v>9.0066983199999999</v>
       </c>
       <c r="E3">
-        <v>18.884555120000002</v>
+        <v>16.745552969999999</v>
       </c>
       <c r="F3">
-        <v>1.9493204500000001</v>
+        <v>4.3820769400000001</v>
+      </c>
+      <c r="G3">
+        <v>15.310256620000001</v>
+      </c>
+      <c r="H3">
+        <v>2.50698321</v>
+      </c>
+      <c r="I3">
+        <v>5.0186043700000003</v>
+      </c>
+      <c r="J3">
+        <v>0.33179396</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>19.60745704</v>
+      </c>
+      <c r="D4">
+        <v>8.4163074800000004</v>
+      </c>
+      <c r="E4">
+        <v>14.55165423</v>
+      </c>
+      <c r="F4">
+        <v>3.29758928</v>
+      </c>
+      <c r="G4">
+        <v>9.7910599000000005</v>
+      </c>
+      <c r="H4">
+        <v>2.3804757599999999</v>
+      </c>
+      <c r="I4">
+        <v>5.0709115100000002</v>
+      </c>
+      <c r="J4">
+        <v>0.48098058999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>16.495111999999999</v>
+      </c>
+      <c r="D5">
+        <v>4.1341109200000004</v>
+      </c>
+      <c r="E5">
+        <v>13.07396301</v>
+      </c>
+      <c r="F5">
+        <v>1.82039157</v>
+      </c>
+      <c r="G5">
+        <v>7.65384726</v>
+      </c>
+      <c r="H5">
+        <v>2.0119502200000001</v>
+      </c>
+      <c r="I5">
+        <v>5.62253413</v>
+      </c>
+      <c r="J5">
+        <v>0.80904396000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>12.560255870000001</v>
+      </c>
+      <c r="D6">
+        <v>2.6713778499999998</v>
+      </c>
+      <c r="E6">
+        <v>12.267059919999999</v>
+      </c>
+      <c r="F6">
+        <v>2.2874768599999999</v>
+      </c>
+      <c r="G6">
+        <v>6.3517459499999998</v>
+      </c>
+      <c r="H6">
+        <v>1.71292113</v>
+      </c>
+      <c r="I6">
+        <v>5.44861621</v>
+      </c>
+      <c r="J6">
+        <v>0.69452316000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>10.630800929999999</v>
+      </c>
+      <c r="D7">
+        <v>2.1866767199999999</v>
+      </c>
+      <c r="E7">
+        <v>10.625191170000001</v>
+      </c>
+      <c r="F7">
+        <v>2.9333133600000001</v>
+      </c>
+      <c r="G7">
+        <v>5.8024258800000004</v>
+      </c>
+      <c r="H7">
+        <v>0.86696993</v>
+      </c>
+      <c r="I7">
+        <v>5.5629818899999997</v>
+      </c>
+      <c r="J7">
+        <v>0.64764542999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>8.7671184400000008</v>
+      </c>
+      <c r="D8">
+        <v>0.98441886000000001</v>
+      </c>
+      <c r="E8">
+        <v>8.2254345299999994</v>
+      </c>
+      <c r="F8">
+        <v>1.32651864</v>
+      </c>
+      <c r="G8">
+        <v>5.1452005999999999</v>
+      </c>
+      <c r="H8">
+        <v>0.67946207999999997</v>
+      </c>
+      <c r="I8">
+        <v>5.11745961</v>
+      </c>
+      <c r="J8">
+        <v>0.83527476000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>8.2256209600000005</v>
+      </c>
+      <c r="D9">
+        <v>1.79769348</v>
+      </c>
+      <c r="E9">
+        <v>6.9714984299999996</v>
+      </c>
+      <c r="F9">
+        <v>2.4107172299999999</v>
+      </c>
+      <c r="G9">
+        <v>4.8134608500000002</v>
+      </c>
+      <c r="H9">
+        <v>0.83370027999999996</v>
+      </c>
+      <c r="I9">
+        <v>4.6668473500000003</v>
+      </c>
+      <c r="J9">
+        <v>0.91118546</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>6.6788861199999996</v>
+      </c>
+      <c r="D10">
+        <v>0.70903373999999997</v>
+      </c>
+      <c r="E10">
+        <v>4.75171762</v>
+      </c>
+      <c r="F10">
+        <v>1.66211799</v>
+      </c>
+      <c r="G10">
+        <v>3.87561651</v>
+      </c>
+      <c r="H10">
+        <v>0.84365343999999998</v>
+      </c>
+      <c r="I10">
+        <v>3.8429390899999998</v>
+      </c>
+      <c r="J10">
+        <v>0.92278433999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>